<commit_message>
ques 2 pivote table
</commit_message>
<xml_diff>
--- a/projet final excel.xlsx
+++ b/projet final excel.xlsx
@@ -1,31 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BBA7C3-01B9-41AF-999E-B0063F507272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BACE91-25C4-47FC-A6A6-9F2C26EED945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1C2E421" hidden="1">Sheet1!$C$2:$E$42</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Range" name="Range" connection="WorksheetConnection_Sheet1!$C$2:$E$42"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{9971D317-C2EF-4BCA-BBEF-A7B399FE5C24}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="8" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" xr16:uid="{AE220195-EBE4-4E40-A45F-E830A9DE7C30}" name="WorksheetConnection_Sheet1!$C$2:$E$42" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Range" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1C2E421"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="23">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -42,85 +83,58 @@
     <t>Arts</t>
   </si>
   <si>
-    <t xml:space="preserve"> Yale</t>
-  </si>
-  <si>
     <t>Physics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brown</t>
   </si>
   <si>
     <t>Economics</t>
   </si>
   <si>
-    <t xml:space="preserve"> Dartmouth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Economics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Harvard</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cornell</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Harvard </t>
-  </si>
-  <si>
     <t>Mathematics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Princeton</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mathematics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brown </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dartmouth </t>
   </si>
   <si>
     <t>Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve"> Penn State </t>
-  </si>
-  <si>
     <t>Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Physics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cornell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yale </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columbia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Princeton </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Penn State</t>
   </si>
   <si>
     <t xml:space="preserve">Penn State </t>
   </si>
   <si>
-    <t xml:space="preserve"> Arts</t>
+    <t>Row Labels</t>
   </si>
   <si>
-    <t xml:space="preserve"> Psychology</t>
+    <t>Sum of Students</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Average of Students</t>
+  </si>
+  <si>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>Princeton</t>
+  </si>
+  <si>
+    <t>Dartmouth</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>Penn State</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -225,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,12 +256,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,6 +282,693 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="RAM Tech" refreshedDate="45289.437863310188" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="40" xr:uid="{8F00C3A8-17FD-40F3-BE63-264F5D9D5AB3}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C2:E42" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Students" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="135" maxValue="9567"/>
+    </cacheField>
+    <cacheField name="Faculty" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Arts"/>
+        <s v="Physics"/>
+        <s v="Economics"/>
+        <s v="Mathematics"/>
+        <s v="Psychology"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="University" numFmtId="0">
+      <sharedItems count="16">
+        <s v=" Yale"/>
+        <s v=" Brown"/>
+        <s v=" Dartmouth"/>
+        <s v=" Harvard"/>
+        <s v=" Columbia"/>
+        <s v=" Cornell"/>
+        <s v=" Harvard "/>
+        <s v=" Princeton"/>
+        <s v=" Brown "/>
+        <s v=" Dartmouth "/>
+        <s v=" Penn State "/>
+        <s v=" Cornell "/>
+        <s v=" Yale "/>
+        <s v=" Columbia "/>
+        <s v=" Princeton "/>
+        <s v=" Penn State"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="RAM Tech" refreshedDate="45289.461474074073" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D595849C-0650-4585-98FB-00ECB031227B}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="3">
+    <cacheField name="[Measures].[Sum of Students]" caption="Sum of Students" numFmtId="0" hierarchy="5" level="32767"/>
+    <cacheField name="[Measures].[Average of Students]" caption="Average of Students" numFmtId="0" hierarchy="6" level="32767"/>
+    <cacheField name="[Range].[University].[University]" caption="University" numFmtId="0" hierarchy="2" level="1">
+      <sharedItems count="8">
+        <s v="Brown"/>
+        <s v="Columbia"/>
+        <s v="Cornell"/>
+        <s v="Dartmouth"/>
+        <s v="Harvard"/>
+        <s v="Penn State"/>
+        <s v="Princeton"/>
+        <s v="Yale"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="7">
+    <cacheHierarchy uniqueName="[Range].[Students]" caption="Students" attribute="1" defaultMemberUniqueName="[Range].[Students].[All]" allUniqueName="[Range].[Students].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Faculty]" caption="Faculty" attribute="1" defaultMemberUniqueName="[Range].[Faculty].[All]" allUniqueName="[Range].[Faculty].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[University]" caption="University" attribute="1" defaultMemberUniqueName="[Range].[University].[All]" allUniqueName="[Range].[University].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Range]" caption="__XL_Count Range" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Students]" caption="Sum of Students" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Students]" caption="Average of Students" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Range" uniqueName="[Range]" caption="Range"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Range" caption="Range"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="RAM Tech" refreshedDate="45289.463532175927" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{518AACDC-133B-465C-A573-9280F2722062}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="3">
+    <cacheField name="[Measures].[Sum of Students]" caption="Sum of Students" numFmtId="0" hierarchy="5" level="32767"/>
+    <cacheField name="[Range].[University].[University]" caption="University" numFmtId="0" hierarchy="2" level="1">
+      <sharedItems count="8">
+        <s v="Brown"/>
+        <s v="Columbia"/>
+        <s v="Cornell"/>
+        <s v="Dartmouth"/>
+        <s v="Harvard"/>
+        <s v="Penn State"/>
+        <s v="Princeton"/>
+        <s v="Yale"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Range].[Faculty].[Faculty]" caption="Faculty" numFmtId="0" hierarchy="1" level="1">
+      <sharedItems count="5">
+        <s v="Arts"/>
+        <s v="Economics"/>
+        <s v="Mathematics"/>
+        <s v="Physics"/>
+        <s v="Psychology"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="7">
+    <cacheHierarchy uniqueName="[Range].[Students]" caption="Students" attribute="1" defaultMemberUniqueName="[Range].[Students].[All]" allUniqueName="[Range].[Students].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Faculty]" caption="Faculty" attribute="1" defaultMemberUniqueName="[Range].[Faculty].[All]" allUniqueName="[Range].[Faculty].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Range].[University]" caption="University" attribute="1" defaultMemberUniqueName="[Range].[University].[All]" allUniqueName="[Range].[University].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Range]" caption="__XL_Count Range" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Students]" caption="Sum of Students" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Students]" caption="Average of Students" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Range" uniqueName="[Range]" caption="Range"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Range" caption="Range"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
+  <r>
+    <n v="591"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9567"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="542"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="346"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="849"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="552"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="173"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="1355"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="193"/>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="615"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="1579"/>
+    <x v="3"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="547"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="1687"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="972"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="234"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="151"/>
+    <x v="4"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="1793"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="315"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="618"/>
+    <x v="1"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="246"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="784"/>
+    <x v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="316"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="3155"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="318"/>
+    <x v="4"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="608"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="561"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="357"/>
+    <x v="4"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="1688"/>
+    <x v="3"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="972"/>
+    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <n v="568"/>
+    <x v="1"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="632"/>
+    <x v="3"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="551"/>
+    <x v="4"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="948"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="1358"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="135"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="849"/>
+    <x v="3"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="158"/>
+    <x v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="1889"/>
+    <x v="3"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="651"/>
+    <x v="4"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="651"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0300E900-1E78-404F-8DFA-A29260F90953}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotHierarchies count="7">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="2"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="1"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Sheet1!$C$2:$E$42">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{810373F6-3B2A-4C7C-82C0-74F225AB5177}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotHierarchies count="7">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="2"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Sheet1!$C$2:$E$42">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E42AE1-0578-41CD-B9E2-9BA7FA269454}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students" fld="0" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,11 +1233,500 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76734544-DFD0-454F-924C-EA58BDD23D7D}">
+  <dimension ref="A3:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1358</v>
+      </c>
+      <c r="C5" s="10">
+        <v>972</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1579</v>
+      </c>
+      <c r="E5" s="10">
+        <v>9567</v>
+      </c>
+      <c r="F5" s="10">
+        <v>651</v>
+      </c>
+      <c r="G5" s="10">
+        <v>14127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10">
+        <v>849</v>
+      </c>
+      <c r="C6" s="10">
+        <v>608</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1688</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1793</v>
+      </c>
+      <c r="F6" s="10">
+        <v>315</v>
+      </c>
+      <c r="G6" s="10">
+        <v>5253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1355</v>
+      </c>
+      <c r="C7" s="10">
+        <v>552</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1889</v>
+      </c>
+      <c r="E7" s="10">
+        <v>618</v>
+      </c>
+      <c r="F7" s="10">
+        <v>551</v>
+      </c>
+      <c r="G7" s="10">
+        <v>4965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10">
+        <v>3155</v>
+      </c>
+      <c r="C8" s="10">
+        <v>542</v>
+      </c>
+      <c r="D8" s="10">
+        <v>316</v>
+      </c>
+      <c r="E8" s="10">
+        <v>547</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1687</v>
+      </c>
+      <c r="G8" s="10">
+        <v>6247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10">
+        <v>173</v>
+      </c>
+      <c r="C9" s="10">
+        <v>346</v>
+      </c>
+      <c r="D9" s="10">
+        <v>615</v>
+      </c>
+      <c r="E9" s="10">
+        <v>948</v>
+      </c>
+      <c r="F9" s="10">
+        <v>158</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10">
+        <v>135</v>
+      </c>
+      <c r="C10" s="10">
+        <v>234</v>
+      </c>
+      <c r="D10" s="10">
+        <v>632</v>
+      </c>
+      <c r="E10" s="10">
+        <v>568</v>
+      </c>
+      <c r="F10" s="10">
+        <v>318</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10">
+        <v>561</v>
+      </c>
+      <c r="C11" s="10">
+        <v>972</v>
+      </c>
+      <c r="D11" s="10">
+        <v>193</v>
+      </c>
+      <c r="E11" s="10">
+        <v>784</v>
+      </c>
+      <c r="F11" s="10">
+        <v>151</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="10">
+        <v>591</v>
+      </c>
+      <c r="C12" s="10">
+        <v>651</v>
+      </c>
+      <c r="D12" s="10">
+        <v>849</v>
+      </c>
+      <c r="E12" s="10">
+        <v>246</v>
+      </c>
+      <c r="F12" s="10">
+        <v>357</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10">
+        <v>8177</v>
+      </c>
+      <c r="C13" s="10">
+        <v>4877</v>
+      </c>
+      <c r="D13" s="10">
+        <v>7761</v>
+      </c>
+      <c r="E13" s="10">
+        <v>15071</v>
+      </c>
+      <c r="F13" s="10">
+        <v>4188</v>
+      </c>
+      <c r="G13" s="10">
+        <v>40074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09B551F-E2C5-4F07-8ED4-AB6EF6E779D2}">
+  <dimension ref="A3:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.6328125" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>14127</v>
+      </c>
+      <c r="C4">
+        <v>2825.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>5253</v>
+      </c>
+      <c r="C5">
+        <v>1050.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>4965</v>
+      </c>
+      <c r="C6">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>6247</v>
+      </c>
+      <c r="C7">
+        <v>1249.4000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2240</v>
+      </c>
+      <c r="C8">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1887</v>
+      </c>
+      <c r="C9">
+        <v>377.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>2661</v>
+      </c>
+      <c r="C10">
+        <v>532.20000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2694</v>
+      </c>
+      <c r="C11">
+        <v>538.79999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>40074</v>
+      </c>
+      <c r="C12">
+        <v>1001.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E97646-48B2-4F33-AA8D-589F0EEA10C5}">
+  <dimension ref="A3:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="41.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8177</v>
+      </c>
+      <c r="C4">
+        <v>1022.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4877</v>
+      </c>
+      <c r="C5">
+        <v>609.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7761</v>
+      </c>
+      <c r="C6">
+        <v>970.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>15071</v>
+      </c>
+      <c r="C7">
+        <v>1883.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>4188</v>
+      </c>
+      <c r="C8">
+        <v>523.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>40074</v>
+      </c>
+      <c r="C9">
+        <v>1001.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,11 +1738,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
@@ -568,7 +1763,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.35">
@@ -576,10 +1771,10 @@
         <v>9567</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.35">
@@ -587,10 +1782,10 @@
         <v>542</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.35">
@@ -598,10 +1793,10 @@
         <v>346</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.35">
@@ -612,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.35">
@@ -620,10 +1815,10 @@
         <v>552</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.35">
@@ -634,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.35">
@@ -645,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.35">
@@ -653,10 +1848,10 @@
         <v>193</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.35">
@@ -664,10 +1859,10 @@
         <v>615</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.35">
@@ -675,10 +1870,10 @@
         <v>1579</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.35">
@@ -686,10 +1881,10 @@
         <v>547</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.35">
@@ -697,10 +1892,10 @@
         <v>1687</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.35">
@@ -708,10 +1903,10 @@
         <v>972</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
@@ -719,10 +1914,10 @@
         <v>234</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
@@ -730,10 +1925,10 @@
         <v>151</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
@@ -741,10 +1936,10 @@
         <v>1793</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
@@ -752,10 +1947,10 @@
         <v>315</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.35">
@@ -763,10 +1958,10 @@
         <v>618</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
@@ -774,10 +1969,10 @@
         <v>246</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.35">
@@ -785,10 +1980,10 @@
         <v>784</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.35">
@@ -796,10 +1991,10 @@
         <v>316</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.35">
@@ -810,7 +2005,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
@@ -818,7 +2013,7 @@
         <v>318</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>21</v>
@@ -829,10 +2024,10 @@
         <v>608</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.35">
@@ -843,7 +2038,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.35">
@@ -851,10 +2046,10 @@
         <v>357</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.35">
@@ -862,10 +2057,10 @@
         <v>1688</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.35">
@@ -873,10 +2068,10 @@
         <v>972</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.35">
@@ -884,10 +2079,10 @@
         <v>568</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.35">
@@ -895,10 +2090,10 @@
         <v>632</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.35">
@@ -906,10 +2101,10 @@
         <v>551</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.35">
@@ -917,10 +2112,10 @@
         <v>948</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.35">
@@ -931,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.35">
@@ -939,10 +2134,10 @@
         <v>135</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
@@ -950,10 +2145,10 @@
         <v>849</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
@@ -961,10 +2156,10 @@
         <v>158</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
@@ -972,10 +2167,10 @@
         <v>1889</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.35">
@@ -983,10 +2178,10 @@
         <v>651</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.35">
@@ -994,10 +2189,10 @@
         <v>651</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ques 3 la condition
</commit_message>
<xml_diff>
--- a/projet final excel.xlsx
+++ b/projet final excel.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BACE91-25C4-47FC-A6A6-9F2C26EED945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CEF952-4EED-4BAB-A4EC-28E18002A00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlcn.WorksheetConnection_Sheet1C2E421" hidden="1">Sheet1!$C$2:$E$42</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
-    <pivotCache cacheId="7" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,6 +38,15 @@
           <x15:modelTable id="Range" name="Range" connection="WorksheetConnection_Sheet1!$C$2:$E$42"/>
         </x15:modelTables>
       </x15:dataModel>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -66,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="34">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -135,13 +145,49 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>QTE</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>Remise</t>
+  </si>
+  <si>
+    <t>Val Remise</t>
+  </si>
+  <si>
+    <t>Total a payer</t>
+  </si>
+  <si>
+    <t>total Facture :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val TVA </t>
+  </si>
+  <si>
+    <t>TVA :</t>
+  </si>
+  <si>
+    <t>TTC :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_([$DZD]\ * #,##0.00_);_([$DZD]\ * \(#,##0.00\);_([$DZD]\ * &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +211,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +259,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -235,11 +315,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,10 +430,75 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -687,7 +916,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0300E900-1E78-404F-8DFA-A29260F90953}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0300E900-1E78-404F-8DFA-A29260F90953}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -905,7 +1134,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E42AE1-0578-41CD-B9E2-9BA7FA269454}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E42AE1-0578-41CD-B9E2-9BA7FA269454}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -1233,10 +1462,473 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD5E5AA-7CCE-41F6-ABAF-F48EB46BF28B}">
+  <dimension ref="B3:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" customWidth="1"/>
+    <col min="8" max="8" width="23.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27">
+        <v>120</v>
+      </c>
+      <c r="D4" s="28">
+        <v>3</v>
+      </c>
+      <c r="E4" s="22">
+        <f>D4*C4</f>
+        <v>360</v>
+      </c>
+      <c r="F4" s="15">
+        <f>IF(E4&gt;=1000,1/10,IF(E4&gt;=100,5/100,0))</f>
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="22">
+        <f>E4*F4</f>
+        <v>18</v>
+      </c>
+      <c r="H4" s="22">
+        <f>E4-G4</f>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29">
+        <v>56</v>
+      </c>
+      <c r="D5" s="30">
+        <v>5</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" ref="E5:E17" si="0">D5*C5</f>
+        <v>280</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" ref="F5:F17" si="1">IF(E5&gt;=1000,1/10,IF(E5&gt;=100,5/100,0))</f>
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" ref="G5:G17" si="2">E5*F5</f>
+        <v>14</v>
+      </c>
+      <c r="H5" s="23">
+        <f t="shared" ref="H5:H17" si="3">E5-G5</f>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="11">
+        <v>3</v>
+      </c>
+      <c r="C6" s="27">
+        <v>70</v>
+      </c>
+      <c r="D6" s="28">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="G6" s="22">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="29">
+        <v>430</v>
+      </c>
+      <c r="D7" s="30">
+        <v>7</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>3010</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="2"/>
+        <v>301</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" si="3"/>
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="11">
+        <v>5</v>
+      </c>
+      <c r="C8" s="27">
+        <v>230</v>
+      </c>
+      <c r="D8" s="28">
+        <v>23</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" si="0"/>
+        <v>5290</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="22">
+        <f t="shared" si="2"/>
+        <v>529</v>
+      </c>
+      <c r="H8" s="22">
+        <f t="shared" si="3"/>
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="12">
+        <v>6</v>
+      </c>
+      <c r="C9" s="29">
+        <v>10</v>
+      </c>
+      <c r="D9" s="30">
+        <v>2</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="11">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27">
+        <v>5</v>
+      </c>
+      <c r="D10" s="28">
+        <v>8</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="22">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="29">
+        <v>5040</v>
+      </c>
+      <c r="D11" s="30">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="2"/>
+        <v>504</v>
+      </c>
+      <c r="H11" s="23">
+        <f t="shared" si="3"/>
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="11">
+        <v>9</v>
+      </c>
+      <c r="C12" s="27">
+        <v>1200</v>
+      </c>
+      <c r="D12" s="28">
+        <v>3</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+      <c r="H12" s="22">
+        <f t="shared" si="3"/>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="29">
+        <v>480</v>
+      </c>
+      <c r="D13" s="30">
+        <v>4</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>1920</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="11">
+        <v>11</v>
+      </c>
+      <c r="C14" s="27">
+        <v>33</v>
+      </c>
+      <c r="D14" s="28">
+        <v>5</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="2"/>
+        <v>8.25</v>
+      </c>
+      <c r="H14" s="22">
+        <f t="shared" si="3"/>
+        <v>156.75</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="12">
+        <v>12</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1200</v>
+      </c>
+      <c r="D15" s="30">
+        <v>2</v>
+      </c>
+      <c r="E15" s="23">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="3"/>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="11">
+        <v>13</v>
+      </c>
+      <c r="C16" s="27">
+        <v>15</v>
+      </c>
+      <c r="D16" s="28">
+        <v>10</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="H16" s="22">
+        <f t="shared" si="3"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="18">
+        <v>14</v>
+      </c>
+      <c r="C17" s="31">
+        <v>24</v>
+      </c>
+      <c r="D17" s="32">
+        <v>5</v>
+      </c>
+      <c r="E17" s="24">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F17" s="19">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="24">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H17" s="24">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E18" s="25"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="33">
+        <f>SUM(H4:H17)</f>
+        <v>20348.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="21">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="33">
+        <f>I19*I20</f>
+        <v>3866.1675</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="H22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="34">
+        <f>I19+I21</f>
+        <v>24214.4175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76734544-DFD0-454F-924C-EA58BDD23D7D}">
   <dimension ref="A3:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1286,22 +1978,22 @@
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>1358</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <v>972</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5">
         <v>1579</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5">
         <v>9567</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5">
         <v>651</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5">
         <v>14127</v>
       </c>
     </row>
@@ -1309,22 +2001,22 @@
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>849</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6">
         <v>608</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>1688</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6">
         <v>1793</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6">
         <v>315</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6">
         <v>5253</v>
       </c>
     </row>
@@ -1332,22 +2024,22 @@
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7">
         <v>1355</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <v>552</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <v>1889</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7">
         <v>618</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7">
         <v>551</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7">
         <v>4965</v>
       </c>
     </row>
@@ -1355,22 +2047,22 @@
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>3155</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <v>542</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8">
         <v>316</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8">
         <v>547</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8">
         <v>1687</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8">
         <v>6247</v>
       </c>
     </row>
@@ -1378,22 +2070,22 @@
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9">
         <v>173</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9">
         <v>346</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9">
         <v>615</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9">
         <v>948</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9">
         <v>158</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9">
         <v>2240</v>
       </c>
     </row>
@@ -1401,22 +2093,22 @@
       <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10">
         <v>135</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10">
         <v>234</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10">
         <v>632</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10">
         <v>568</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10">
         <v>318</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10">
         <v>1887</v>
       </c>
     </row>
@@ -1424,22 +2116,22 @@
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11">
         <v>561</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11">
         <v>972</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11">
         <v>193</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11">
         <v>784</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11">
         <v>151</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11">
         <v>2661</v>
       </c>
     </row>
@@ -1447,22 +2139,22 @@
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12">
         <v>591</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12">
         <v>651</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
         <v>849</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12">
         <v>246</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12">
         <v>357</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12">
         <v>2694</v>
       </c>
     </row>
@@ -1470,22 +2162,22 @@
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13">
         <v>8177</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13">
         <v>4877</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13">
         <v>7761</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13">
         <v>15071</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13">
         <v>4188</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13">
         <v>40074</v>
       </c>
     </row>
@@ -1494,7 +2186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09B551F-E2C5-4F07-8ED4-AB6EF6E779D2}">
   <dimension ref="A3:C12"/>
   <sheetViews>
@@ -1624,7 +2316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E97646-48B2-4F33-AA8D-589F0EEA10C5}">
   <dimension ref="A3:C9"/>
   <sheetViews>
@@ -1721,7 +2413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:E42"/>
   <sheetViews>

</xml_diff>

<commit_message>
ques 4 les graph
</commit_message>
<xml_diff>
--- a/projet final excel.xlsx
+++ b/projet final excel.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CEF952-4EED-4BAB-A4EC-28E18002A00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5FB250-16FA-4BFB-835D-7F526BD58506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="8" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlcn.WorksheetConnection_Sheet1C2E421" hidden="1">Sheet1!$C$2:$E$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="37">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -179,6 +180,15 @@
   <si>
     <t>TTC :</t>
   </si>
+  <si>
+    <t>Distance (m)</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Speed (m/s)</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$DZD]\ * #,##0.00_);_([$DZD]\ * \(#,##0.00\);_([$DZD]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +243,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +285,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -423,12 +446,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -451,7 +468,6 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -471,7 +487,7 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,6 +511,36 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,6 +557,2461 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> / Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet6!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-34F0-4D20-852B-678AFAE766F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="141487055"/>
+        <c:axId val="348398383"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$D$2:$D$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>Speed (m/s)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.666666667</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6.75</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7.4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>8.166666667</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9.375</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9.222222222</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>9.1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$B$3:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$B$3:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-34F0-4D20-852B-678AFAE766F0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Distance (m)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$B$3:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$C$3:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>91</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-34F0-4D20-852B-678AFAE766F0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="141487055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348398383"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348398383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="141487055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed / distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet6!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5A7B-4E04-80DF-46A407E8BCBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distance (m)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5A7B-4E04-80DF-46A407E8BCBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="667357087"/>
+        <c:axId val="668203311"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Distance (m)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$C$4:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>91</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet6!$C$3:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>91</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-5A7B-4E04-80DF-46A407E8BCBA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="667357087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="668203311"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="668203311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667357087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38905249343832021"/>
+          <c:y val="0.88946704578594338"/>
+          <c:w val="0.23381714785651794"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1034E872-16BE-67D8-8C35-B952234086DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{714B74A2-CF68-93B9-305C-3B839278C653}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1462,10 +3963,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FF8667-8584-482E-BCC0-93C5023234FC}">
+  <dimension ref="B2:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="34">
+        <v>1</v>
+      </c>
+      <c r="C3" s="35">
+        <v>5</v>
+      </c>
+      <c r="D3" s="35">
+        <f>C3/B3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="36">
+        <v>2</v>
+      </c>
+      <c r="C4" s="37">
+        <v>10</v>
+      </c>
+      <c r="D4" s="37">
+        <f t="shared" ref="D4:D11" si="0">C4/B4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="34">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35">
+        <v>17</v>
+      </c>
+      <c r="D5" s="35">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="36">
+        <v>4</v>
+      </c>
+      <c r="C6" s="37">
+        <v>27</v>
+      </c>
+      <c r="D6" s="37">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="34">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35">
+        <v>37</v>
+      </c>
+      <c r="D7" s="35">
+        <f t="shared" si="0"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="36">
+        <v>6</v>
+      </c>
+      <c r="C8" s="37">
+        <v>49</v>
+      </c>
+      <c r="D8" s="37">
+        <f t="shared" si="0"/>
+        <v>8.1666666666666661</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="34">
+        <v>7</v>
+      </c>
+      <c r="C9" s="35">
+        <v>63</v>
+      </c>
+      <c r="D9" s="35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="36">
+        <v>8</v>
+      </c>
+      <c r="C10" s="37">
+        <v>75</v>
+      </c>
+      <c r="D10" s="37">
+        <f t="shared" si="0"/>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="34">
+        <v>9</v>
+      </c>
+      <c r="C11" s="35">
+        <v>83</v>
+      </c>
+      <c r="D11" s="35">
+        <f t="shared" si="0"/>
+        <v>9.2222222222222214</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="38">
+        <v>10</v>
+      </c>
+      <c r="C12" s="39">
+        <v>91</v>
+      </c>
+      <c r="D12" s="39">
+        <f>C12/B12</f>
+        <v>9.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD5E5AA-7CCE-41F6-ABAF-F48EB46BF28B}">
   <dimension ref="B3:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -1480,441 +4132,440 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="24">
         <v>120</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="25">
         <v>3</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="19">
         <f>D4*C4</f>
         <v>360</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <f>IF(E4&gt;=1000,1/10,IF(E4&gt;=100,5/100,0))</f>
         <v>0.05</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="19">
         <f>E4*F4</f>
         <v>18</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="19">
         <f>E4-G4</f>
         <v>342</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="26">
         <v>56</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="27">
         <v>5</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <f t="shared" ref="E5:E17" si="0">D5*C5</f>
         <v>280</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <f t="shared" ref="F5:F17" si="1">IF(E5&gt;=1000,1/10,IF(E5&gt;=100,5/100,0))</f>
         <v>0.05</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <f t="shared" ref="G5:G17" si="2">E5*F5</f>
         <v>14</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="20">
         <f t="shared" ref="H5:H17" si="3">E5-G5</f>
         <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="24">
         <v>70</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>2</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="19">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <f t="shared" si="3"/>
         <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="26">
         <v>430</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="27">
         <v>7</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <f t="shared" si="0"/>
         <v>3010</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="14">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <f t="shared" si="2"/>
         <v>301</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="20">
         <f t="shared" si="3"/>
         <v>2709</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="24">
         <v>230</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="25">
         <v>23</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="19">
         <f t="shared" si="0"/>
         <v>5290</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="19">
         <f t="shared" si="2"/>
         <v>529</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="19">
         <f t="shared" si="3"/>
         <v>4761</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="26">
         <v>10</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="27">
         <v>2</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="20">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="24">
         <v>5</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="25">
         <v>8</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="19">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="19">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>8</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="26">
         <v>5040</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="27">
         <v>1</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="14">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <f t="shared" si="2"/>
         <v>504</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="20">
         <f t="shared" si="3"/>
         <v>4536</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="24">
         <v>1200</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>3</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="19">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="13">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="19">
         <f t="shared" si="2"/>
         <v>360</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="19">
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>10</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="26">
         <v>480</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="27">
         <v>4</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="14">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="20">
         <f t="shared" si="3"/>
         <v>1728</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="11">
+      <c r="B14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="24">
         <v>33</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="25">
         <v>5</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="19">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="13">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="19">
         <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="19">
         <f t="shared" si="3"/>
         <v>156.75</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="26">
         <v>1200</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="27">
         <v>2</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="14">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="20">
         <f t="shared" si="3"/>
         <v>2160</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="11">
+      <c r="B16" s="9">
         <v>13</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="24">
         <v>15</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="25">
         <v>10</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="19">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="19">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="19">
         <f t="shared" si="3"/>
         <v>142.5</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="18">
+      <c r="B17" s="15">
         <v>14</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="28">
         <v>24</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="29">
         <v>5</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="21">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="21">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="E18" s="25"/>
-      <c r="F18" s="17"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="30">
         <f>SUM(H4:H17)</f>
         <v>20348.25</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="18">
         <v>0.19</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="30">
         <f>I19*I20</f>
         <v>3866.1675</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.5">
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="31">
         <f>I19+I21</f>
         <v>24214.4175</v>
       </c>
@@ -1924,7 +4575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76734544-DFD0-454F-924C-EA58BDD23D7D}">
   <dimension ref="A3:G13"/>
   <sheetViews>
@@ -2186,7 +4837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09B551F-E2C5-4F07-8ED4-AB6EF6E779D2}">
   <dimension ref="A3:C12"/>
   <sheetViews>
@@ -2316,7 +4967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E97646-48B2-4F33-AA8D-589F0EEA10C5}">
   <dimension ref="A3:C9"/>
   <sheetViews>
@@ -2413,7 +5064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:E42"/>
   <sheetViews>
@@ -2430,11 +5081,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">

</xml_diff>